<commit_message>
Updated list to include decryption profiles
</commit_message>
<xml_diff>
--- a/docs/checklists/Iron-Skillet-Checklist.xlsx
+++ b/docs/checklists/Iron-Skillet-Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtelan/Documents/pstools/threat-reports/docs/checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AF7F48-0E30-6641-8BEF-2F90D350A910}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEED17B-D40D-6448-B885-619EDADE3AA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{14F8B973-F82A-3442-84B7-FC7F22DA6A5A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{14F8B973-F82A-3442-84B7-FC7F22DA6A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="NGFW" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="231">
   <si>
     <t>Change</t>
   </si>
@@ -649,9 +649,6 @@
     <t>Iron-Skillet creates a Recommended_Decryption_Profile with approprate settings.  Settings are as follows</t>
   </si>
   <si>
-    <t>SSL Decryption Tab</t>
-  </si>
-  <si>
     <t>SSL Forward Proxy Check</t>
   </si>
   <si>
@@ -659,30 +656,6 @@
   </si>
   <si>
     <t>SSL Protocol Settings</t>
-  </si>
-  <si>
-    <t>Min version TLSv1.2</t>
-  </si>
-  <si>
-    <t>Key Exhange Algorithms Disable RSA, Enable DHE and ECDHE</t>
-  </si>
-  <si>
-    <t>Encryption Algorithms Disable 3DES and RC4, Enable all others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Authentication Algorithms </t>
-  </si>
-  <si>
-    <t>Enable SHA256 and SHA384, Disable SHA1 and MD5</t>
-  </si>
-  <si>
-    <t>No Decyrption</t>
-  </si>
-  <si>
-    <t>Enable Block sessions with expired certificates and Block sessioins with untrusted issuers</t>
-  </si>
-  <si>
-    <t>SSH Proxy</t>
   </si>
   <si>
     <t>Zone Protection</t>
@@ -840,6 +813,51 @@
   </si>
   <si>
     <t>Rematch session will force current sessions to rematch when security policy is commited</t>
+  </si>
+  <si>
+    <t>SSL Decryption</t>
+  </si>
+  <si>
+    <t>No Decryption Policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSH Proxy  </t>
+  </si>
+  <si>
+    <t>Objects &gt; Decryption &gt; Decryption Profile &gt; SSL Decryption</t>
+  </si>
+  <si>
+    <t>Objects &gt; Decryption &gt; Decryption Profile &gt; SSL Decryption &gt; SSL Forward Proxy</t>
+  </si>
+  <si>
+    <t>SSL Inbound Inspection</t>
+  </si>
+  <si>
+    <t>Objects &gt; Decryption &gt; Decryption Profile &gt; SSL Decryption &gt; SSL Inbound Inspection</t>
+  </si>
+  <si>
+    <t>No Changes required</t>
+  </si>
+  <si>
+    <t>Objects &gt; Decryption &gt; Decryption Profile &gt; SSL Decryption &gt; SSL Protocol Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objects &gt; Decryption &gt; Decryption Profile &gt; No Decryption </t>
+  </si>
+  <si>
+    <t>Objects &gt; Decryption &gt; Decryption Profile &gt; SSH Proxy</t>
+  </si>
+  <si>
+    <t>Enable Block sessions with expired certificates and Enable Block sessioins with untrusted issuers</t>
+  </si>
+  <si>
+    <t>Enable Block sessions with unsupported sessions and Enable Block sessioins with unsupported algorithms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Exhange Algorithms Disable RSA, Enable DHE and ECDHE, Encryption Algorithms Disable 3DES and RC4, Enable all others, </t>
+  </si>
+  <si>
+    <t>Min version TLSv1.2, Key Exhange Algorithms Disable RSA, Enable DHE and ECDHE, Encryption Algorithms Disable 3DES and RC4, Enable all others, Encryption Algorithms Disable 3DES and RC4, enable all others, Enable SHA256 and SHA384, Disable SHA1 and MD5, Enable SHA256 and SHA384, Disable SHA1 and MD5</t>
   </si>
 </sst>
 </file>
@@ -898,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -910,6 +928,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1225,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEC0790-7940-F441-838A-7934F4C2F489}">
-  <dimension ref="A1:F112"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,7 +1341,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1499,13 +1520,13 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D32" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1997,136 +2018,140 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D87" s="1" t="s">
+      <c r="B87" t="s">
+        <v>216</v>
+      </c>
+      <c r="C87" t="s">
+        <v>219</v>
+      </c>
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D88" s="1" t="s">
+      <c r="C88" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D88" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>221</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>222</v>
+      </c>
       <c r="D89" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B90" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D90" s="1" t="s">
-        <v>177</v>
+      <c r="C90" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>217</v>
+      </c>
+      <c r="C91" t="s">
+        <v>225</v>
+      </c>
       <c r="D91" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D92" t="s">
-        <v>179</v>
+      <c r="B92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" t="s">
+        <v>226</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" t="s">
+        <v>179</v>
+      </c>
+      <c r="D95" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D94" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
         <v>181</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D95" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D96" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D97" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D98" s="1" t="s">
+      <c r="C99" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D99" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C102" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D102" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D103" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D104" t="s">
+      <c r="A104" s="1" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="1" t="s">
+      <c r="B105" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
-        <v>193</v>
-      </c>
-      <c r="C106" t="s">
-        <v>194</v>
-      </c>
-      <c r="D106" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
-        <v>197</v>
-      </c>
-      <c r="C109" t="s">
-        <v>198</v>
-      </c>
-      <c r="D109" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B112" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2141,7 +2166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF54FE3-5C89-1E43-B6CE-B387B65B1C4A}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2322,7 +2347,7 @@
         <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D21" t="s">
         <v>91</v>
@@ -2333,7 +2358,7 @@
         <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -2344,7 +2369,7 @@
         <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D23" t="s">
         <v>99</v>
@@ -2355,7 +2380,7 @@
         <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D24" t="s">
         <v>100</v>
@@ -2366,7 +2391,7 @@
         <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="D25" t="s">
         <v>106</v>
@@ -2377,7 +2402,7 @@
         <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D26" t="s">
         <v>107</v>
@@ -2388,7 +2413,7 @@
         <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D27" t="s">
         <v>112</v>
@@ -2396,24 +2421,24 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C28" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" t="s">
         <v>209</v>
-      </c>
-      <c r="D28" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" t="s">
         <v>210</v>
-      </c>
-      <c r="C29" t="s">
-        <v>211</v>
-      </c>
-      <c r="D29" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2421,10 +2446,10 @@
         <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2432,30 +2457,30 @@
         <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D31" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C32" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D32" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C33" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D33" t="s">
         <v>99</v>
@@ -2463,13 +2488,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C34" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D34" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated panos assessment reports IS checklist and added instructions
</commit_message>
<xml_diff>
--- a/docs/checklists/Iron-Skillet-Checklist.xlsx
+++ b/docs/checklists/Iron-Skillet-Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtelan/Documents/pstools/threat-reports/docs/checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEED17B-D40D-6448-B885-619EDADE3AA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6A4720-0FBC-084B-8026-5770F11B39CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{14F8B973-F82A-3442-84B7-FC7F22DA6A5A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="235">
   <si>
     <t>Change</t>
   </si>
@@ -670,52 +670,6 @@
     <t>Iron-Skillet will create a "Recommended_Zone_Protection" profiles which includes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Reconnaissance Protection</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Enable TCP Port Scan, Host Sweep, and UDP Port Scan</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Packet Based Attack Protection</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - Enable Spoofed IP Address and Malformed</t>
-    </r>
-  </si>
-  <si>
     <t>Security Profiles</t>
   </si>
   <si>
@@ -858,6 +812,24 @@
   </si>
   <si>
     <t>Min version TLSv1.2, Key Exhange Algorithms Disable RSA, Enable DHE and ECDHE, Encryption Algorithms Disable 3DES and RC4, Enable all others, Encryption Algorithms Disable 3DES and RC4, enable all others, Enable SHA256 and SHA384, Disable SHA1 and MD5, Enable SHA256 and SHA384, Disable SHA1 and MD5</t>
+  </si>
+  <si>
+    <t>Reconnaissance Protection</t>
+  </si>
+  <si>
+    <t>Network &gt; Network Profiles &gt; Zone Protection &gt; Reconnaissance Protection</t>
+  </si>
+  <si>
+    <t>Enable TCP Port Scan, Host Sweep, and UDP Port Scan</t>
+  </si>
+  <si>
+    <t>Packet Based Attack Protection</t>
+  </si>
+  <si>
+    <t>Network &gt; Network Profiles &gt; Zone Protection &gt; Packet Based Attack Protection</t>
+  </si>
+  <si>
+    <t>Enable Spoofed IP Address and Malformed</t>
   </si>
 </sst>
 </file>
@@ -927,10 +899,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1248,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCEC0790-7940-F441-838A-7934F4C2F489}">
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1341,7 +1313,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1479,7 +1451,7 @@
       <c r="D27" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F27" t="s">
@@ -1496,7 +1468,7 @@
       <c r="D28" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="6"/>
       <c r="F28" t="s">
         <v>68</v>
       </c>
@@ -1520,13 +1492,13 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D32" t="s">
         <v>213</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D32" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2019,10 +1991,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C87" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D87" s="1"/>
     </row>
@@ -2030,8 +2002,8 @@
       <c r="B88" t="s">
         <v>174</v>
       </c>
-      <c r="C88" s="6" t="s">
-        <v>220</v>
+      <c r="C88" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>175</v>
@@ -2039,51 +2011,51 @@
     </row>
     <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="C89" s="6" t="s">
+    </row>
+    <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B90" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C90" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D89" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="B90" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>224</v>
-      </c>
       <c r="D90" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C91" t="s">
+        <v>223</v>
+      </c>
+      <c r="D91" t="s">
         <v>225</v>
-      </c>
-      <c r="D91" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C92" t="s">
+        <v>224</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2103,55 +2075,67 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
+        <v>229</v>
+      </c>
+      <c r="C96" t="s">
+        <v>230</v>
+      </c>
       <c r="D96" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>232</v>
+      </c>
+      <c r="C97" t="s">
+        <v>233</v>
+      </c>
       <c r="D97" t="s">
-        <v>182</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" t="s">
         <v>184</v>
-      </c>
-      <c r="C99" t="s">
-        <v>185</v>
-      </c>
-      <c r="D99" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
+        <v>186</v>
+      </c>
+      <c r="C102" t="s">
+        <v>187</v>
+      </c>
+      <c r="D102" t="s">
         <v>188</v>
-      </c>
-      <c r="C102" t="s">
-        <v>189</v>
-      </c>
-      <c r="D102" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2347,7 +2331,7 @@
         <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D21" t="s">
         <v>91</v>
@@ -2358,7 +2342,7 @@
         <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
         <v>95</v>
@@ -2369,7 +2353,7 @@
         <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D23" t="s">
         <v>99</v>
@@ -2380,7 +2364,7 @@
         <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
         <v>100</v>
@@ -2391,7 +2375,7 @@
         <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D25" t="s">
         <v>106</v>
@@ -2402,7 +2386,7 @@
         <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D26" t="s">
         <v>107</v>
@@ -2413,7 +2397,7 @@
         <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D27" t="s">
         <v>112</v>
@@ -2421,24 +2405,24 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2446,10 +2430,10 @@
         <v>123</v>
       </c>
       <c r="C30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2457,30 +2441,30 @@
         <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D31" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D33" t="s">
         <v>99</v>
@@ -2488,13 +2472,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C34" t="s">
+        <v>204</v>
+      </c>
+      <c r="D34" t="s">
         <v>206</v>
-      </c>
-      <c r="D34" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>